<commit_message>
OW-965, updated the algo input parameters
</commit_message>
<xml_diff>
--- a/test/testCallAmount/callAmountPerformance.xlsx
+++ b/test/testCallAmount/callAmountPerformance.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="5">
   <si>
     <t>x</t>
   </si>
@@ -88,7 +88,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="298">
+  <cellXfs count="366">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
@@ -141,6 +141,210 @@
       <alignment wrapText="true"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
       <alignment wrapText="true"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
@@ -992,275 +1196,275 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="230" t="s">
+      <c r="A1" s="298" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="231" t="s">
+      <c r="B1" s="299" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="232" t="n">
+      <c r="A2" s="300" t="n">
         <v>5000.0</v>
       </c>
-      <c r="B2" s="233" t="n">
+      <c r="B2" s="301" t="n">
         <v>0.020000000000436557</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="234" t="n">
+      <c r="A3" s="302" t="n">
         <v>10000.0</v>
       </c>
-      <c r="B3" s="235" t="n">
+      <c r="B3" s="303" t="n">
         <v>0.010000000002037268</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="236" t="n">
+      <c r="A4" s="304" t="n">
         <v>15000.0</v>
       </c>
-      <c r="B4" s="237" t="n">
+      <c r="B4" s="305" t="n">
+        <v>0.00999999999839929</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="306" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="B5" s="307" t="n">
+        <v>0.01999999999679858</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="308" t="n">
+        <v>25000.0</v>
+      </c>
+      <c r="B6" s="309" t="n">
+        <v>0.049999999999272404</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="310" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="B7" s="311" t="n">
         <v>0.020000000000436557</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="238" t="n">
-        <v>20000.0</v>
-      </c>
-      <c r="B5" s="239" t="n">
+    <row r="8">
+      <c r="A8" s="312" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="B8" s="313" t="n">
+        <v>0.030000000002473826</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="314" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="B9" s="315" t="n">
+        <v>0.020000000000436557</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="316" t="n">
+        <v>45000.0</v>
+      </c>
+      <c r="B10" s="317" t="n">
+        <v>0.020000000000436557</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="318" t="n">
+        <v>50000.0</v>
+      </c>
+      <c r="B11" s="319" t="n">
+        <v>0.020000000000436557</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="320" t="n">
+        <v>55000.0</v>
+      </c>
+      <c r="B12" s="321" t="n">
         <v>0.010000000002037268</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="240" t="n">
-        <v>25000.0</v>
-      </c>
-      <c r="B6" s="241" t="n">
+    <row r="13">
+      <c r="A13" s="322" t="n">
+        <v>60000.0</v>
+      </c>
+      <c r="B13" s="323" t="n">
         <v>0.020000000000436557</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="242" t="n">
-        <v>30000.0</v>
-      </c>
-      <c r="B7" s="243" t="n">
+    <row r="14">
+      <c r="A14" s="324" t="n">
+        <v>65000.0</v>
+      </c>
+      <c r="B14" s="325" t="n">
+        <v>0.00999999999839929</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="326" t="n">
+        <v>70000.0</v>
+      </c>
+      <c r="B15" s="327" t="n">
         <v>0.020000000000436557</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="244" t="n">
-        <v>35000.0</v>
-      </c>
-      <c r="B8" s="245" t="n">
-        <v>0.010000000002037268</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="246" t="n">
-        <v>40000.0</v>
-      </c>
-      <c r="B9" s="247" t="n">
+    <row r="16">
+      <c r="A16" s="328" t="n">
+        <v>75000.0</v>
+      </c>
+      <c r="B16" s="329" t="n">
+        <v>0.00999999999839929</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="330" t="n">
+        <v>80000.0</v>
+      </c>
+      <c r="B17" s="331" t="n">
+        <v>0.01999999999679858</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="332" t="n">
+        <v>85000.0</v>
+      </c>
+      <c r="B18" s="333" t="n">
+        <v>0.00999999999839929</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="334" t="n">
+        <v>90000.0</v>
+      </c>
+      <c r="B19" s="335" t="n">
+        <v>0.030000000002473826</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="336" t="n">
+        <v>95000.0</v>
+      </c>
+      <c r="B20" s="337" t="n">
         <v>0.020000000000436557</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="248" t="n">
-        <v>45000.0</v>
-      </c>
-      <c r="B10" s="249" t="n">
-        <v>0.020000000000436557</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="250" t="n">
-        <v>50000.0</v>
-      </c>
-      <c r="B11" s="251" t="n">
+    <row r="21">
+      <c r="A21" s="338" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="B21" s="339" t="n">
+        <v>0.040000000000873115</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="340" t="n">
+        <v>105000.0</v>
+      </c>
+      <c r="B22" s="341" t="n">
+        <v>0.029999999998835847</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="342" t="n">
+        <v>110000.0</v>
+      </c>
+      <c r="B23" s="343" t="n">
+        <v>0.040000000000873115</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="344" t="n">
+        <v>115000.0</v>
+      </c>
+      <c r="B24" s="345" t="n">
+        <v>0.029999999998835847</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="346" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="B25" s="347" t="n">
+        <v>0.029999999998835847</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="348" t="n">
+        <v>125000.0</v>
+      </c>
+      <c r="B26" s="349" t="n">
+        <v>0.06000000000130967</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="350" t="n">
+        <v>130000.0</v>
+      </c>
+      <c r="B27" s="351" t="n">
+        <v>0.040000000000873115</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="352" t="n">
+        <v>135000.0</v>
+      </c>
+      <c r="B28" s="353" t="n">
+        <v>0.030000000002473826</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="354" t="n">
+        <v>140000.0</v>
+      </c>
+      <c r="B29" s="355" t="n">
         <v>0.049999999999272404</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="252" t="n">
-        <v>55000.0</v>
-      </c>
-      <c r="B12" s="253" t="n">
-        <v>0.010000000002037268</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="254" t="n">
-        <v>60000.0</v>
-      </c>
-      <c r="B13" s="255" t="n">
-        <v>0.020000000000436557</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="256" t="n">
-        <v>65000.0</v>
-      </c>
-      <c r="B14" s="257" t="n">
-        <v>0.030000000002473826</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="258" t="n">
-        <v>70000.0</v>
-      </c>
-      <c r="B15" s="259" t="n">
-        <v>0.020000000000436557</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="260" t="n">
-        <v>75000.0</v>
-      </c>
-      <c r="B16" s="261" t="n">
+    <row r="30">
+      <c r="A30" s="356" t="n">
+        <v>145000.0</v>
+      </c>
+      <c r="B30" s="357" t="n">
+        <v>0.040000000000873115</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="358" t="n">
+        <v>150000.0</v>
+      </c>
+      <c r="B31" s="359" t="n">
+        <v>0.049999999999272404</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="360" t="n">
+        <v>155000.0</v>
+      </c>
+      <c r="B32" s="361" t="n">
         <v>0.029999999998835847</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="262" t="n">
-        <v>80000.0</v>
-      </c>
-      <c r="B17" s="263" t="n">
-        <v>0.030000000002473826</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="264" t="n">
-        <v>85000.0</v>
-      </c>
-      <c r="B18" s="265" t="n">
-        <v>0.049999999999272404</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="266" t="n">
-        <v>90000.0</v>
-      </c>
-      <c r="B19" s="267" t="n">
-        <v>0.020000000000436557</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="268" t="n">
-        <v>95000.0</v>
-      </c>
-      <c r="B20" s="269" t="n">
-        <v>0.00999999999839929</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="270" t="n">
-        <v>100000.0</v>
-      </c>
-      <c r="B21" s="271" t="n">
+    <row r="33">
+      <c r="A33" s="362" t="n">
+        <v>160000.0</v>
+      </c>
+      <c r="B33" s="363" t="n">
         <v>0.029999999998835847</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="272" t="n">
-        <v>105000.0</v>
-      </c>
-      <c r="B22" s="273" t="n">
+    <row r="34">
+      <c r="A34" s="364" t="n">
+        <v>165000.0</v>
+      </c>
+      <c r="B34" s="365" t="n">
         <v>0.029999999998835847</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="274" t="n">
-        <v>110000.0</v>
-      </c>
-      <c r="B23" s="275" t="n">
-        <v>0.049999999999272404</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="276" t="n">
-        <v>115000.0</v>
-      </c>
-      <c r="B24" s="277" t="n">
-        <v>0.040000000000873115</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="278" t="n">
-        <v>120000.0</v>
-      </c>
-      <c r="B25" s="279" t="n">
-        <v>0.029999999998835847</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="280" t="n">
-        <v>125000.0</v>
-      </c>
-      <c r="B26" s="281" t="n">
-        <v>0.040000000000873115</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="282" t="n">
-        <v>130000.0</v>
-      </c>
-      <c r="B27" s="283" t="n">
-        <v>0.030000000002473826</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="284" t="n">
-        <v>135000.0</v>
-      </c>
-      <c r="B28" s="285" t="n">
-        <v>0.029999999998835847</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="286" t="n">
-        <v>140000.0</v>
-      </c>
-      <c r="B29" s="287" t="n">
-        <v>0.029999999998835847</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="288" t="n">
-        <v>145000.0</v>
-      </c>
-      <c r="B30" s="289" t="n">
-        <v>0.030000000002473826</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="290" t="n">
-        <v>150000.0</v>
-      </c>
-      <c r="B31" s="291" t="n">
-        <v>0.040000000000873115</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="292" t="n">
-        <v>155000.0</v>
-      </c>
-      <c r="B32" s="293" t="n">
-        <v>0.029999999998835847</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="294" t="n">
-        <v>160000.0</v>
-      </c>
-      <c r="B33" s="295" t="n">
-        <v>0.030000000002473826</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="296" t="n">
-        <v>165000.0</v>
-      </c>
-      <c r="B34" s="297" t="n">
-        <v>0.040000000000873115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>